<commit_message>
Genericinun model with transport ready including animation. Density not yet.
</commit_message>
<xml_diff>
--- a/Projects/VoortoetsAGT/cases/GenericInun/GenericInun.xlsx
+++ b/Projects/VoortoetsAGT/cases/GenericInun/GenericInun.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/VoortoetsAGT/cases/GenericInun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D2CD63-8C94-9249-BBBC-F874B511FF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3360C767-F425-FD4D-B7D3-55A022612F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11860" yWindow="-26760" windowWidth="30600" windowHeight="19860" tabRatio="751" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2488" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="409">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1356,9 +1356,6 @@
     <t>Solver for Gwt</t>
   </si>
   <si>
-    <t>MODERATE</t>
-  </si>
-  <si>
     <t>SIMPLE | MODERATE | COMPLEX</t>
   </si>
   <si>
@@ -1431,13 +1428,10 @@
     <t>khaki</t>
   </si>
   <si>
-    <t>A0000</t>
-  </si>
-  <si>
-    <t>Inundatielaag</t>
-  </si>
-  <si>
-    <t>lightgray</t>
+    <t>COMPLEX</t>
+  </si>
+  <si>
+    <t>Split</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +1562,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1590,6 +1584,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1976,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2112,11 +2107,11 @@
         <v>268</v>
       </c>
       <c r="B9" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>269</v>
@@ -2397,11 +2392,11 @@
         <v>381</v>
       </c>
       <c r="B28" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="12" t="str">
         <f t="shared" ref="C28" si="1">IF(B28=1,"&lt;====","")</f>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>382</v>
@@ -2412,11 +2407,11 @@
         <v>306</v>
       </c>
       <c r="B29" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>307</v>
@@ -2442,11 +2437,11 @@
         <v>310</v>
       </c>
       <c r="B31" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>311</v>
@@ -2487,11 +2482,11 @@
         <v>316</v>
       </c>
       <c r="B34" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>317</v>
@@ -2517,11 +2512,11 @@
         <v>320</v>
       </c>
       <c r="B36" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>321</v>
@@ -2562,11 +2557,11 @@
         <v>326</v>
       </c>
       <c r="B39" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>327</v>
@@ -2622,11 +2617,11 @@
         <v>334</v>
       </c>
       <c r="B43" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>335</v>
@@ -2667,11 +2662,11 @@
         <v>340</v>
       </c>
       <c r="B46" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="12" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>341</v>
@@ -2697,11 +2692,11 @@
         <v>378</v>
       </c>
       <c r="B48" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="12" t="str">
         <f>IF(B48=1,"&lt;====","")</f>
-        <v/>
+        <v>&lt;====</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>376</v>
@@ -3552,8 +3547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView topLeftCell="A7" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3678,10 +3673,10 @@
         <v>111</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -3779,8 +3774,8 @@
       <c r="B20" t="s">
         <v>120</v>
       </c>
-      <c r="C20" t="s">
-        <v>22</v>
+      <c r="C20">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -3889,8 +3884,8 @@
       <c r="B30" t="s">
         <v>130</v>
       </c>
-      <c r="C30" t="s">
-        <v>22</v>
+      <c r="C30">
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -4308,7 +4303,7 @@
         <v>48</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -5730,7 +5725,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A209" t="s">
         <v>347</v>
       </c>
@@ -5741,7 +5736,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A210" t="s">
         <v>347</v>
       </c>
@@ -5752,7 +5747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A211" t="s">
         <v>347</v>
       </c>
@@ -5763,7 +5758,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A212" t="s">
         <v>347</v>
       </c>
@@ -5774,7 +5769,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A213" t="s">
         <v>347</v>
       </c>
@@ -5785,7 +5780,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A214" t="s">
         <v>347</v>
       </c>
@@ -5796,7 +5791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A215" t="s">
         <v>347</v>
       </c>
@@ -5807,7 +5802,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A216" t="s">
         <v>347</v>
       </c>
@@ -5818,7 +5813,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A217" t="s">
         <v>347</v>
       </c>
@@ -5829,7 +5824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A218" t="s">
         <v>347</v>
       </c>
@@ -5837,10 +5832,13 @@
         <v>46</v>
       </c>
       <c r="C218" s="11" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.15">
+        <v>398</v>
+      </c>
+      <c r="D218" s="11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A219" t="s">
         <v>347</v>
       </c>
@@ -5851,7 +5849,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A221" t="s">
         <v>276</v>
       </c>
@@ -5862,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A222" t="s">
         <v>276</v>
       </c>
@@ -5873,7 +5871,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A223" t="s">
         <v>276</v>
       </c>
@@ -5884,7 +5882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A224" t="s">
         <v>276</v>
       </c>
@@ -8535,8 +8533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06ADD67-459A-3448-A388-0C190A7D0288}">
   <dimension ref="A1:D315"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A16" zoomScale="203" zoomScaleNormal="203" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8701,10 +8699,10 @@
         <v>111</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -8802,8 +8800,8 @@
       <c r="B24" t="s">
         <v>120</v>
       </c>
-      <c r="C24" t="s">
-        <v>22</v>
+      <c r="C24">
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -8912,8 +8910,8 @@
       <c r="B34" t="s">
         <v>130</v>
       </c>
-      <c r="C34" t="s">
-        <v>22</v>
+      <c r="C34">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
@@ -11844,10 +11842,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11893,18 +11891,624 @@
         <v>45292</v>
       </c>
       <c r="C3" s="10">
-        <f>DATE(2054,1,1)-DATE(2024,1,1)</f>
-        <v>10958</v>
+        <v>365</v>
       </c>
       <c r="D3" s="10">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C4" s="10">
+        <v>365</v>
+      </c>
+      <c r="D4" s="10">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C5" s="10">
+        <v>365</v>
+      </c>
+      <c r="D5" s="10">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C6" s="10">
+        <v>365</v>
+      </c>
+      <c r="D6" s="10">
+        <v>12</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C7" s="10">
+        <v>365</v>
+      </c>
+      <c r="D7" s="10">
+        <v>12</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C8" s="10">
+        <v>365</v>
+      </c>
+      <c r="D8" s="10">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C9" s="10">
+        <v>365</v>
+      </c>
+      <c r="D9" s="10">
+        <v>12</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C10" s="10">
+        <v>365</v>
+      </c>
+      <c r="D10" s="10">
+        <v>12</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C11" s="10">
+        <v>365</v>
+      </c>
+      <c r="D11" s="10">
+        <v>12</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C12" s="10">
+        <v>365</v>
+      </c>
+      <c r="D12" s="10">
+        <v>12</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C13" s="10">
+        <v>365</v>
+      </c>
+      <c r="D13" s="10">
+        <v>12</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C14" s="10">
+        <v>365</v>
+      </c>
+      <c r="D14" s="10">
+        <v>12</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C15" s="10">
+        <v>365</v>
+      </c>
+      <c r="D15" s="10">
+        <v>12</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C16" s="10">
+        <v>365</v>
+      </c>
+      <c r="D16" s="10">
+        <v>12</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C17" s="10">
+        <v>365</v>
+      </c>
+      <c r="D17" s="10">
+        <v>12</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C18" s="10">
+        <v>365</v>
+      </c>
+      <c r="D18" s="10">
+        <v>12</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C19" s="10">
+        <v>365</v>
+      </c>
+      <c r="D19" s="10">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C20" s="10">
+        <v>365</v>
+      </c>
+      <c r="D20" s="10">
+        <v>12</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C21" s="10">
+        <v>365</v>
+      </c>
+      <c r="D21" s="10">
+        <v>12</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C22" s="10">
+        <v>365</v>
+      </c>
+      <c r="D22" s="10">
+        <v>12</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C23" s="10">
+        <v>365</v>
+      </c>
+      <c r="D23" s="10">
+        <v>12</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C24" s="10">
+        <v>365</v>
+      </c>
+      <c r="D24" s="10">
+        <v>12</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C25" s="10">
+        <v>365</v>
+      </c>
+      <c r="D25" s="10">
+        <v>12</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C26" s="10">
+        <v>365</v>
+      </c>
+      <c r="D26" s="10">
+        <v>12</v>
+      </c>
+      <c r="E26" s="10">
+        <v>1</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C27" s="10">
+        <v>365</v>
+      </c>
+      <c r="D27" s="10">
+        <v>12</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C28" s="10">
+        <v>365</v>
+      </c>
+      <c r="D28" s="10">
+        <v>12</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C29" s="10">
+        <v>365</v>
+      </c>
+      <c r="D29" s="10">
+        <v>12</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C30" s="10">
+        <v>365</v>
+      </c>
+      <c r="D30" s="10">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C31" s="10">
+        <v>365</v>
+      </c>
+      <c r="D31" s="10">
+        <v>12</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C32" s="10">
+        <v>365</v>
+      </c>
+      <c r="D32" s="10">
+        <v>12</v>
+      </c>
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33">
         <v>30</v>
       </c>
-      <c r="E3" s="10">
-        <v>1.25</v>
-      </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
+      <c r="B33" s="15">
+        <v>45292</v>
+      </c>
+      <c r="C33" s="10">
+        <v>365</v>
+      </c>
+      <c r="D33" s="10">
+        <v>12</v>
+      </c>
+      <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B34" s="15"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11916,20 +12520,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>76</v>
@@ -11938,62 +12542,68 @@
         <v>78</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
       <c r="C2">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>410</v>
+      <c r="G2" s="17">
+        <v>1</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+        <v>392</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>0.2</v>
@@ -12001,28 +12611,31 @@
       <c r="F3" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="17">
+        <v>5</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>0.2</v>
@@ -12030,28 +12643,31 @@
       <c r="F4" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="17">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -12059,72 +12675,49 @@
       <c r="F5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>405</v>
+      <c r="G5" s="17">
+        <v>10</v>
       </c>
       <c r="H5" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>395</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
+      <c r="C6" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1E-3</v>
       </c>
       <c r="E6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F6" s="2">
         <v>1E-4</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="17">
+        <v>5</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>396</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>389</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1E-3</v>
-      </c>
-      <c r="E7">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>